<commit_message>
Course 13 - ExtentManager, ExtentTestManager, ExtentTestListener
</commit_message>
<xml_diff>
--- a/src/test/resources/data/testdata.xlsx
+++ b/src/test/resources/data/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndreiGunta\IdeaProjects\TestProject2024\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{573E01A4-A297-430D-ADDF-EF6E2A2FB7CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71229AAC-6FC0-4AEB-B163-789466EC3B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1188" yWindow="3240" windowWidth="17304" windowHeight="8892" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -498,7 +498,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>